<commit_message>
added id to table
</commit_message>
<xml_diff>
--- a/peilvakken_node_ids.xlsx
+++ b/peilvakken_node_ids.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louiseklingen/code/MargaritaLK/rtcxdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5B49E22-A9DE-7944-832A-1A042ACB926A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E382D4-C5CB-4245-89E2-E223F53064DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15760" yWindow="1380" windowWidth="28040" windowHeight="17440" xr2:uid="{826D19A8-B000-E348-87E2-FB1F720F801D}"/>
+    <workbookView xWindow="5560" yWindow="1380" windowWidth="28040" windowHeight="17440" xr2:uid="{826D19A8-B000-E348-87E2-FB1F720F801D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>peilvak</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>03150-10</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -402,54 +405,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26649545-7F9F-8744-A9A8-932FE9BEFDED}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>29960</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>28303</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>28202</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>27908</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>2364</v>
       </c>
     </row>

</xml_diff>